<commit_message>
add more datasets to run for experiment
</commit_message>
<xml_diff>
--- a/Data Output/ParamSearch_Experiment_evaluation.xlsx
+++ b/Data Output/ParamSearch_Experiment_evaluation.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="ParamSearch_Experiment_evaluati" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="26">
   <si>
     <t>corr_true</t>
   </si>
@@ -99,6 +99,9 @@
   <si>
     <t>Average of decline_slope</t>
   </si>
+  <si>
+    <t>Average of corr_true</t>
+  </si>
 </sst>
 </file>
 
@@ -107,10 +110,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,18 +152,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -619,11 +647,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125432632"/>
-        <c:axId val="-2111397752"/>
+        <c:axId val="-2091251304"/>
+        <c:axId val="-2057788984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125432632"/>
+        <c:axId val="-2091251304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-2111397752"/>
+        <c:crossAx val="-2057788984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -640,7 +668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111397752"/>
+        <c:axId val="-2057788984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,7 +679,532 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-2125432632"/>
+        <c:crossAx val="-2091251304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NewAtEnd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$4:$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nltk_0.20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nltk_0.40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>nltk_0.60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>nltk_0.80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>word2vec_0.20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>word2vec_0.40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>word2vec_0.60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>word2vec_0.80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$5:$U$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.655872083445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.534319190255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.545937901372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.545937901372</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.520048262718</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.717803333497</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.650549604701</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.504343114793</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Exciting</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$4:$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nltk_0.20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nltk_0.40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>nltk_0.60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>nltk_0.80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>word2vec_0.20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>word2vec_0.40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>word2vec_0.60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>word2vec_0.80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$6:$U$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.878335405378</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.824387389218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.820139551059</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.820139551059</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.691770571595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.826027545337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.877400999291</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.831318073622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$4:$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nltk_0.20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nltk_0.40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>nltk_0.60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>nltk_0.80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>word2vec_0.20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>word2vec_0.40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>word2vec_0.60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>word2vec_0.80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$7:$U$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.775512457282</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70018789537</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.723354963509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.723354963509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0892171603884</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4555780352</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.652680112835</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.698651973568</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Boring</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$4:$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nltk_0.20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nltk_0.40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>nltk_0.60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>nltk_0.80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>word2vec_0.20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>word2vec_0.40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>word2vec_0.60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>word2vec_0.80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$8:$U$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.780601012252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.745056074441</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.747353943922</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.747353943922</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.265398731373</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55911736685</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.768067490583</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73593108521</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SuperBoring</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$4:$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nltk_0.20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nltk_0.40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>nltk_0.60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>nltk_0.80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>word2vec_0.20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>word2vec_0.40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>word2vec_0.60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>word2vec_0.80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$9:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.891259969649</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86126283073</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.875023141796</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.875023141796</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.592386624797</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.769541346615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.831387092044</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.874216219759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2085906440"/>
+        <c:axId val="2030088232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2085906440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="2030088232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2030088232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="-2085906440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -675,19 +1228,14 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="11595100" cy="5245100"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -704,7 +1252,34 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="11595100" cy="5245100"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1082,7 +1657,106 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="M3:V10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of corr_true" fld="0" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:J10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1502,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J10"/>
+  <dimension ref="A3:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1515,17 +2189,28 @@
     <col min="3" max="5" width="8.83203125" customWidth="1"/>
     <col min="6" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="M3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1556,8 +2241,38 @@
       <c r="J4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="M4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1588,8 +2303,38 @@
       <c r="J5" s="3">
         <v>-6.7552700922282492E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="M5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.65587208344500003</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0.53431919025499997</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.54593790137200005</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0.54593790137200005</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0.52004826271799998</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0.71780333349699998</v>
+      </c>
+      <c r="T5" s="4">
+        <v>0.65054960470099998</v>
+      </c>
+      <c r="U5" s="4">
+        <v>0.50434311479299998</v>
+      </c>
+      <c r="V5" s="4">
+        <v>0.58435142401912499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1620,8 +2365,38 @@
       <c r="J6" s="3">
         <v>-9.6645256916887516E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="M6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.87833540537800003</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0.82438738921800003</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0.82013955105900005</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0.82013955105900005</v>
+      </c>
+      <c r="R6" s="4">
+        <v>0.69177057159499999</v>
+      </c>
+      <c r="S6" s="4">
+        <v>0.82602754533699996</v>
+      </c>
+      <c r="T6" s="4">
+        <v>0.87740099929100002</v>
+      </c>
+      <c r="U6" s="4">
+        <v>0.83131807362200005</v>
+      </c>
+      <c r="V6" s="4">
+        <v>0.82118988581987495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1652,8 +2427,38 @@
       <c r="J7" s="3">
         <v>-9.5360671936889976E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="M7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.77551245728200002</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0.70018789537000004</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0.72335496350899997</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0.72335496350899997</v>
+      </c>
+      <c r="R7" s="4">
+        <v>8.9217160388399996E-2</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0.45557803520000001</v>
+      </c>
+      <c r="T7" s="4">
+        <v>0.65268011283500005</v>
+      </c>
+      <c r="U7" s="4">
+        <v>0.69865197356800002</v>
+      </c>
+      <c r="V7" s="4">
+        <v>0.60231719520767502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1684,8 +2489,38 @@
       <c r="J8" s="3">
         <v>-7.7663043478304996E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="M8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.78060101225199996</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0.74505607444099997</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.74735394392200005</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0.74735394392200005</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.26539873137300002</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0.55911736685000002</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0.76806749058299995</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0.73593108520999995</v>
+      </c>
+      <c r="V8" s="4">
+        <v>0.66860995606912499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1716,8 +2551,38 @@
       <c r="J9" s="3">
         <v>-8.1506916996137505E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="M9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.89125996964900001</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.86126283072999998</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.87502314179600005</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.87502314179600005</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.59238662479699999</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0.76954134661499995</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0.83138709204399996</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0.87421621975899999</v>
+      </c>
+      <c r="V9" s="4">
+        <v>0.82126254589824998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1748,10 +2613,41 @@
       <c r="J10" s="3">
         <v>-8.3745718050100507E-3</v>
       </c>
+      <c r="M10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.79631618560119999</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0.73304267600279993</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0.74236190033159999</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0.74236190033159999</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.43176427017427998</v>
+      </c>
+      <c r="S10" s="4">
+        <v>0.66561352549980002</v>
+      </c>
+      <c r="T10" s="4">
+        <v>0.75601705989080004</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0.72889209339039995</v>
+      </c>
+      <c r="V10" s="4">
+        <v>0.69954620140280999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>